<commit_message>
Lab 5 code finished
</commit_message>
<xml_diff>
--- a/Non-Code Stuff/Navigation Odo Data.xlsx
+++ b/Non-Code Stuff/Navigation Odo Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="0" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,8 +97,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -139,7 +143,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -152,6 +156,8 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -164,6 +170,8 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,7 +504,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -531,343 +539,343 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2">
-        <f ca="1">RAND()*2.5 + 58.5</f>
-        <v>60.434299846926109</v>
+      <c r="A2" s="3">
+        <f t="shared" ref="A2:C11" ca="1" si="0">RAND()*2.5 - 1</f>
+        <v>0.77411196831914331</v>
       </c>
       <c r="B2" s="3">
         <f ca="1">RAND()*2.5 - 1</f>
-        <v>0.19344638733029207</v>
-      </c>
-      <c r="C2" s="2">
-        <f t="shared" ref="C2:C11" ca="1" si="0">RAND()*2.5 + 58.5</f>
-        <v>60.144571155159326</v>
+        <v>1.0665888919030282</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0098686878676686</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:D11" ca="1" si="1">RAND()*2.5 - 1</f>
-        <v>-0.46161335882634513</v>
+        <v>-0.14433626841627301</v>
       </c>
       <c r="E2" s="3">
         <f ca="1">ABS(A2-C2)</f>
-        <v>0.28972869176678273</v>
+        <v>0.23575671954852528</v>
       </c>
       <c r="F2" s="3">
         <f ca="1">ABS(B2-D2)</f>
-        <v>0.6550597461566372</v>
+        <v>1.2109251603193012</v>
       </c>
       <c r="H2" s="1">
         <f ca="1">(E2-$E$12)^2</f>
-        <v>0.69655083915835769</v>
+        <v>5.3392558984415563E-2</v>
       </c>
       <c r="I2" s="1">
         <f ca="1">(F2-$F$12)^2</f>
-        <v>0.34753525546575048</v>
+        <v>0.21210317096829942</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2">
-        <f t="shared" ref="A3:A12" ca="1" si="2">RAND()*2.5 + 58.5</f>
-        <v>59.362799478528736</v>
+      <c r="A3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.0165756945503883E-3</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ref="B3:B11" ca="1" si="3">RAND()*2.5 - 1</f>
-        <v>0.94544305824787345</v>
-      </c>
-      <c r="C3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>60.464231408573681</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.43473453740126611</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.65147810779899173</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.75816130413829308</v>
+        <v>-5.0322200729150612E-2</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:F11" ca="1" si="4">ABS(A3-C3)</f>
-        <v>1.1014319300449458</v>
+        <f t="shared" ref="E3:F11" ca="1" si="2">ABS(A3-C3)</f>
+        <v>0.66049468349354212</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.7036043623861665</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.3844123366721155</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H11" ca="1" si="5">(E3-$E$12)^2</f>
-        <v>5.2408830270780557E-4</v>
+        <f t="shared" ref="H3:H11" ca="1" si="3">(E3-$E$12)^2</f>
+        <v>3.750793896765512E-2</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I11" ca="1" si="6">(F3-$F$12)^2</f>
-        <v>0.21070248869222363</v>
+        <f t="shared" ref="I3:I11" ca="1" si="4">(F3-$F$12)^2</f>
+        <v>0.13393127669424601</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.820225258856311</v>
+      <c r="A4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.40534317501103723</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>8.8952289481905478E-2</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>59.732814985969497</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.44941739621118759</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.669713145904826</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.88436411184332475</v>
+        <v>1.3184552601035233</v>
       </c>
       <c r="E4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.26436997089378877</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.86903786389233573</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.0988046480048522E-2</v>
+      </c>
+      <c r="I4" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0874102728868138</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.97331640132523023</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>1.3626900647211657E-3</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>7.3584457983562709E-2</v>
+        <v>1.4080030375127253E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.28468826794326</v>
+      <c r="A5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10683459362891701</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.85098403705672387</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>60.711289230793497</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.60377476597037871</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1366982419074243</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72257484032422559</v>
+        <v>0.62636801476662374</v>
       </c>
       <c r="E5" s="3">
-        <f ca="1">ABS(A5-C5)</f>
-        <v>0.42660096285023741</v>
+        <f t="shared" ref="E5:E11" ca="1" si="5">ABS(A5-C5)</f>
+        <v>2.9863648278507293E-2</v>
       </c>
       <c r="F5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.2593248796245025E-2</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.19093523945178373</v>
+      </c>
+      <c r="I5" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5735588773809495</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.48681869946165546</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.1082264735314922</v>
+        <v>0.52967145935781168</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>58.542063360963162</v>
+      <c r="A6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.96374632332127952</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.14134011494138643</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>59.075565596387676</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3776756721121979</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7038515855111207E-2</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.2889295825113667E-3</v>
+        <v>-0.42575465940163415</v>
       </c>
       <c r="E6" s="3">
-        <f ca="1">ABS(A6-C6)</f>
-        <v>0.53350223542451403</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.91670780746616831</v>
       </c>
       <c r="F6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.803430331513832</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.20239452341062597</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.14005118535887506</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.34907142689501591</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>1.2199860116292902</v>
+        <v>1.1089180332657884</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>58.766641706114235</v>
+      <c r="A7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.9571043934870476E-2</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.2561593983943249</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>60.489734660028837</v>
+        <f ca="1">RAND()*2.5 - 1</f>
+        <v>0.57087031616621098</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.45145528854595796</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.79195942955652598</v>
+        <v>-0.30015577208654376</v>
       </c>
       <c r="E7" s="3">
-        <f ca="1">ABS(A7-C7)</f>
-        <v>1.7230929539146018</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.54102633248082843</v>
       </c>
       <c r="F7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.87102608825275474</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.5058349309443306E-3</v>
+      </c>
+      <c r="I7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>2.0481188279508507</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.35852317639014292</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.64567311355314538</v>
+        <v>1.4555826047992482E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.675618753969061</v>
+      <c r="A8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51727949898131387</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.57747715040690739</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>58.980397407962293</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.68520125420550604</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0968155477797836</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0562258156811972</v>
+        <v>0.88930795291757869</v>
       </c>
       <c r="E8" s="3">
-        <f ca="1">ABS(A8-C8)</f>
-        <v>1.6952213460067682</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.57953604879846976</v>
       </c>
       <c r="F8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5745092071230848</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.2703776251392308E-2</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.47874866527428983</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.32592274634384366</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.58649909571321257</v>
+        <v>0.67919132335328047</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.950384541886194</v>
+      <c r="A9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.11198761011087877</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.96447772213180327</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>59.657942781345866</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.075344881488153</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1212088628237287</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.55263816913896724</v>
+        <v>0.99939726198598189</v>
       </c>
       <c r="E9" s="3">
-        <f ca="1">ABS(A9-C9)</f>
-        <v>1.2924417605403278</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.0092212527128499</v>
       </c>
       <c r="F9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.5947619502171104E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.29419367440921773</v>
+      </c>
+      <c r="I9" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5171158912707705</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>2.8263277113719364E-2</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>7.4275291585375658E-2</v>
+        <v>0.45485709364337124</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.760624513404089</v>
+      <c r="A10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0651359249691632</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.29576857918807331</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>58.586904396046613</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.24385633907236026</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3914424877983089</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.301272011064615</v>
+        <v>3.9553662540035006E-2</v>
       </c>
       <c r="E10" s="3">
-        <f ca="1">ABS(A10-C10)</f>
-        <v>2.1737201173574761</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.32630656282914572</v>
       </c>
       <c r="F10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.28341000161239527</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.9745436508232576E-2</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0055034318765417</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>1.1012303116997659</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>5.7158061977525369E-2</v>
+        <v>0.21805963462132225</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>60.964528559372262</v>
+      <c r="A11" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.31987162188636487</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1.4763953421726703</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>60.044429780074076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.53476016269479887</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21490445897201726</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.87433681706261135</v>
+        <v>0.9432539060676417</v>
       </c>
       <c r="E11" s="3">
-        <f ca="1">ABS(A11-C11)</f>
-        <v>0.92009877929818629</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.1049671629143476</v>
       </c>
       <c r="F11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.40849374337284283</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.13094110796865219</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>2.3507321592352817</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>4.1708310422875775E-2</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>1.223570487025929</v>
+        <v>0.11688522791246467</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -879,11 +887,11 @@
       </c>
       <c r="E12" s="4">
         <f ca="1">SUM(E2:E11)/10</f>
-        <v>1.1243249050090653</v>
+        <v>0.46682501894161721</v>
       </c>
       <c r="F12" s="4">
         <f ca="1">SUM(F2:F11)/10</f>
-        <v>1.2445809548215592</v>
+        <v>0.7503785601057078</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -895,11 +903,11 @@
       </c>
       <c r="E13" s="4">
         <f ca="1">(SUM(H2:H11)/10)^(1/2)</f>
-        <v>0.5822349668177621</v>
+        <v>0.31437368486611089</v>
       </c>
       <c r="F13" s="4">
         <f ca="1">(SUM(I2:I11)/10)^(1/2)</f>
-        <v>0.67433009254796772</v>
+        <v>0.5901061833466672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>